<commit_message>
Merged PR 3611: Merge develop_accessible to develop
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ProprietaryDataFiles/Syndication_InvalidFile1.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ProprietaryDataFiles/Syndication_InvalidFile1.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oleksandr\Desktop\data files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\achyzh\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\ProprietaryDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562671D8-6015-4422-89C5-4E4C8D954122}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barter Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -168,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -657,29 +665,29 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
     <dxf>
@@ -1274,12 +1282,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="15" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1339,19 +1347,19 @@
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37" t="str">
+      <c r="D2" s="29"/>
+      <c r="E2" s="35" t="str">
         <f>IF(COUNTA($E$3:$E10) &gt; 0, "Errors", "")</f>
         <v>Errors</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="34"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1376,18 +1384,18 @@
       <c r="B3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="30" t="s">
+      <c r="D3" s="31"/>
+      <c r="E3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="32"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="34"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1410,18 +1418,18 @@
         <v>6</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="30" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="34"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1444,18 +1452,18 @@
         <v>8</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="30" t="s">
+      <c r="D5" s="31"/>
+      <c r="E5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="32"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="34"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1478,18 +1486,18 @@
         <v>9</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="30" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="32"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="34"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1512,16 +1520,16 @@
         <v>11</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="33">
+      <c r="C7" s="30">
         <v>25.123000000000001</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="32"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="34"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1544,16 +1552,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="32"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="34"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1576,16 +1584,16 @@
         <v>14</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="32"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="34"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1608,18 +1616,18 @@
         <v>15</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30" t="s">
+      <c r="D10" s="37"/>
+      <c r="E10" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="34"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1793,7 +1801,9 @@
       <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="19">
+        <v>1</v>
+      </c>
       <c r="C16" s="19">
         <v>0.62</v>
       </c>
@@ -1837,7 +1847,9 @@
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
       <c r="C17" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -1881,7 +1893,9 @@
       <c r="A18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="19">
+        <v>1</v>
+      </c>
       <c r="C18" s="19">
         <v>1.58</v>
       </c>
@@ -1925,7 +1939,9 @@
       <c r="A19" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="19"/>
+      <c r="B19" s="19">
+        <v>1</v>
+      </c>
       <c r="C19" s="19">
         <v>0.56999999999999995</v>
       </c>
@@ -1969,7 +1985,9 @@
       <c r="A20" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="19"/>
+      <c r="B20" s="19">
+        <v>1</v>
+      </c>
       <c r="C20" s="19">
         <v>1</v>
       </c>
@@ -2013,7 +2031,9 @@
       <c r="A21" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="19">
+        <v>1</v>
+      </c>
       <c r="C21" s="19">
         <v>0.78</v>
       </c>
@@ -2057,7 +2077,9 @@
       <c r="A22" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="19"/>
+      <c r="B22" s="19">
+        <v>1</v>
+      </c>
       <c r="C22" s="19">
         <v>0.78</v>
       </c>
@@ -2101,7 +2123,9 @@
       <c r="A23" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="19"/>
+      <c r="B23" s="19">
+        <v>1</v>
+      </c>
       <c r="C23" s="19">
         <v>6.31</v>
       </c>
@@ -2145,7 +2169,9 @@
       <c r="A24" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="19"/>
+      <c r="B24" s="19">
+        <v>1</v>
+      </c>
       <c r="C24" s="19">
         <v>3.34</v>
       </c>
@@ -2189,7 +2215,9 @@
       <c r="A25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="19"/>
+      <c r="B25" s="19">
+        <v>1</v>
+      </c>
       <c r="C25" s="19">
         <v>1.44</v>
       </c>
@@ -2233,7 +2261,9 @@
       <c r="A26" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="19"/>
+      <c r="B26" s="19">
+        <v>1</v>
+      </c>
       <c r="C26" s="19">
         <v>1.42</v>
       </c>
@@ -2277,7 +2307,9 @@
       <c r="A27" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="19"/>
+      <c r="B27" s="19">
+        <v>1</v>
+      </c>
       <c r="C27" s="19">
         <v>0.76</v>
       </c>
@@ -2321,7 +2353,9 @@
       <c r="A28" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="19"/>
+      <c r="B28" s="19">
+        <v>1</v>
+      </c>
       <c r="C28" s="19">
         <v>2.0299999999999998</v>
       </c>
@@ -2365,7 +2399,9 @@
       <c r="A29" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="19"/>
+      <c r="B29" s="19">
+        <v>1</v>
+      </c>
       <c r="C29" s="19">
         <v>1.39</v>
       </c>
@@ -2409,7 +2445,9 @@
       <c r="A30" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="19"/>
+      <c r="B30" s="19">
+        <v>1</v>
+      </c>
       <c r="C30" s="19">
         <v>2.12</v>
       </c>
@@ -2453,7 +2491,9 @@
       <c r="A31" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="19"/>
+      <c r="B31" s="19">
+        <v>1</v>
+      </c>
       <c r="C31" s="19">
         <v>2.29</v>
       </c>
@@ -2497,7 +2537,9 @@
       <c r="A32" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="19">
+        <v>1</v>
+      </c>
       <c r="C32" s="19">
         <v>0.71</v>
       </c>
@@ -2541,7 +2583,9 @@
       <c r="A33" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="19"/>
+      <c r="B33" s="19">
+        <v>1</v>
+      </c>
       <c r="C33" s="19">
         <v>1</v>
       </c>
@@ -2585,7 +2629,9 @@
       <c r="A34" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="19"/>
+      <c r="B34" s="19">
+        <v>1</v>
+      </c>
       <c r="C34" s="19">
         <v>1.1499999999999999</v>
       </c>
@@ -2629,7 +2675,9 @@
       <c r="A35" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="19"/>
+      <c r="B35" s="19">
+        <v>1</v>
+      </c>
       <c r="C35" s="19">
         <v>0.46</v>
       </c>
@@ -29691,6 +29739,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:J3"/>
@@ -29702,13 +29757,6 @@
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="B9">
     <cfRule type="expression" dxfId="27" priority="1">
@@ -29851,19 +29899,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Inventory Source - The inventory source you entered is unknown.  _x000a__x000a_Please select an existing source from the dropdown or contact support to add the inventory source." sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Inventory Source - The inventory source you entered is unknown.  _x000a__x000a_Please select an existing source from the dropdown or contact support to add the inventory source." sqref="B3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"20th Century Fox (Twentieth Century),CBS Synd,NBCU Syn,WB Syn"</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1/1/1</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>B4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Daypart Code - The daypart code you entered is unknown.  _x000a__x000a_Please select an existing daypart code from the dropdown or contact support to add the daypart code." sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Daypart Code - The daypart code you entered is unknown.  _x000a__x000a_Please select an existing daypart code from the dropdown or contact support to add the daypart code." sqref="B6" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"SYN"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Playback Type - The playback type you entered is unknown.  _x000a__x000a_Please select an existing playback type from the dropdown or contact support to add the playback type." sqref="B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Playback Type - The playback type you entered is unknown.  _x000a__x000a_Please select an existing playback type from the dropdown or contact support to add the playback type." sqref="B10" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Live,Live+S,Live+1,Live+3,Live+7"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Merged PR 4361: Merge bugs/PRI11102 to develop
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ProprietaryDataFiles/Syndication_InvalidFile1.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ProprietaryDataFiles/Syndication_InvalidFile1.xlsx
@@ -1,28 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\achyzh\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\ProprietaryDataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\ProprietaryDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562671D8-6015-4422-89C5-4E4C8D954122}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{02225484-A5A3-4266-BCAA-429E879BC94F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barter Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -98,12 +91,6 @@
     <t>Avg HH CPM</t>
   </si>
   <si>
-    <t>P 25-54 Avg Rtg</t>
-  </si>
-  <si>
-    <t>P 25-54 Avg Imps (000)</t>
-  </si>
-  <si>
     <t>P 25-54 VPVH</t>
   </si>
   <si>
@@ -171,6 +158,12 @@
   </si>
   <si>
     <t>NBCU Syn</t>
+  </si>
+  <si>
+    <t>Avg P 25-54 Rtg</t>
+  </si>
+  <si>
+    <t>Avg P 25-54 Imps (000)</t>
   </si>
 </sst>
 </file>
@@ -665,26 +658,26 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1287,7 +1280,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="15" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1347,19 +1340,19 @@
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="35" t="str">
+      <c r="D2" s="36"/>
+      <c r="E2" s="37" t="str">
         <f>IF(COUNTA($E$3:$E10) &gt; 0, "Errors", "")</f>
         <v>Errors</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="34"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1382,20 +1375,20 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="34"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1418,18 +1411,18 @@
         <v>6</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="34"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="32"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1452,18 +1445,18 @@
         <v>8</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="34"/>
+      <c r="E5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="34"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="32"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1486,18 +1479,18 @@
         <v>9</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="34"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="32"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1520,16 +1513,16 @@
         <v>11</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="30">
+      <c r="C7" s="33">
         <v>25.123000000000001</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1552,16 +1545,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="32"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1584,16 +1577,16 @@
         <v>14</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1616,18 +1609,18 @@
         <v>15</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="32" t="s">
+      <c r="D10" s="29"/>
+      <c r="E10" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="32"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1776,16 +1769,16 @@
         <v>22</v>
       </c>
       <c r="F15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="I15" s="24" t="s">
         <v>24</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>26</v>
       </c>
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
@@ -1799,7 +1792,7 @@
     </row>
     <row r="16" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="19">
         <v>1</v>
@@ -1845,7 +1838,7 @@
     </row>
     <row r="17" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -1891,7 +1884,7 @@
     </row>
     <row r="18" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18" s="19">
         <v>1</v>
@@ -1937,7 +1930,7 @@
     </row>
     <row r="19" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" s="19">
         <v>1</v>
@@ -1983,7 +1976,7 @@
     </row>
     <row r="20" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="19">
         <v>1</v>
@@ -2029,7 +2022,7 @@
     </row>
     <row r="21" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="19">
         <v>1</v>
@@ -2075,7 +2068,7 @@
     </row>
     <row r="22" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" s="19">
         <v>1</v>
@@ -2121,7 +2114,7 @@
     </row>
     <row r="23" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" s="19">
         <v>1</v>
@@ -2167,7 +2160,7 @@
     </row>
     <row r="24" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24" s="19">
         <v>1</v>
@@ -2213,7 +2206,7 @@
     </row>
     <row r="25" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B25" s="19">
         <v>1</v>
@@ -2259,7 +2252,7 @@
     </row>
     <row r="26" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" s="19">
         <v>1</v>
@@ -2305,7 +2298,7 @@
     </row>
     <row r="27" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" s="19">
         <v>1</v>
@@ -2351,7 +2344,7 @@
     </row>
     <row r="28" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="19">
         <v>1</v>
@@ -2397,7 +2390,7 @@
     </row>
     <row r="29" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" s="19">
         <v>1</v>
@@ -2443,7 +2436,7 @@
     </row>
     <row r="30" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B30" s="19">
         <v>1</v>
@@ -2489,7 +2482,7 @@
     </row>
     <row r="31" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B31" s="19">
         <v>1</v>
@@ -2535,7 +2528,7 @@
     </row>
     <row r="32" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B32" s="19">
         <v>1</v>
@@ -2581,7 +2574,7 @@
     </row>
     <row r="33" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B33" s="19">
         <v>1</v>
@@ -2627,7 +2620,7 @@
     </row>
     <row r="34" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B34" s="19">
         <v>1</v>
@@ -2673,7 +2666,7 @@
     </row>
     <row r="35" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B35" s="19">
         <v>1</v>
@@ -29739,13 +29732,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:J3"/>
@@ -29757,6 +29743,13 @@
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="B9">
     <cfRule type="expression" dxfId="27" priority="1">

</xml_diff>